<commit_message>
Mise a jour des format d'export
</commit_message>
<xml_diff>
--- a/backend/public/DTS_CNSS.xlsx
+++ b/backend/public/DTS_CNSS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Joel\sega\backend\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\joel\sega\backend\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D8A6C30-1358-4BF8-ABCD-B90B69B11652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA00B281-F229-401A-A02B-90A3F52717E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1208,6 +1208,36 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="33" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="29" xfId="30" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1301,9 +1331,6 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="33" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="24" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1362,33 +1389,6 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="28" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="29" xfId="30" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2011,7 +2011,7 @@
   <dimension ref="A9:Q34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="A10" sqref="A10:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2051,12 +2051,12 @@
       <c r="P9" s="1"/>
     </row>
     <row r="10" spans="1:16" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="64" t="s">
+      <c r="A10" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="64"/>
-      <c r="C10" s="64"/>
-      <c r="D10" s="64"/>
+      <c r="B10" s="74"/>
+      <c r="C10" s="74"/>
+      <c r="D10" s="74"/>
       <c r="E10" s="5" t="s">
         <v>9</v>
       </c>
@@ -2079,10 +2079,10 @@
       <c r="P10" s="1"/>
     </row>
     <row r="11" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="77" t="s">
+      <c r="A11" s="87" t="s">
         <v>64</v>
       </c>
-      <c r="B11" s="78"/>
+      <c r="B11" s="88"/>
       <c r="C11" s="13"/>
       <c r="D11" s="2"/>
       <c r="E11" s="24" t="s">
@@ -2101,20 +2101,20 @@
       <c r="J11" s="1"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
-      <c r="M11" s="61" t="s">
+      <c r="M11" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="N11" s="62"/>
-      <c r="O11" s="62"/>
-      <c r="P11" s="63"/>
+      <c r="N11" s="72"/>
+      <c r="O11" s="72"/>
+      <c r="P11" s="73"/>
     </row>
     <row r="12" spans="1:16" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="64" t="s">
+      <c r="A12" s="74" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="64"/>
-      <c r="C12" s="64"/>
-      <c r="D12" s="64"/>
+      <c r="B12" s="74"/>
+      <c r="C12" s="74"/>
+      <c r="D12" s="74"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="1"/>
@@ -2123,20 +2123,20 @@
       <c r="J12" s="1"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
-      <c r="M12" s="65" t="s">
+      <c r="M12" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="N12" s="66"/>
-      <c r="O12" s="66"/>
-      <c r="P12" s="67"/>
+      <c r="N12" s="76"/>
+      <c r="O12" s="76"/>
+      <c r="P12" s="77"/>
     </row>
     <row r="13" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="68" t="s">
+      <c r="A13" s="78" t="s">
         <v>65</v>
       </c>
-      <c r="B13" s="69"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="69"/>
+      <c r="B13" s="79"/>
+      <c r="C13" s="79"/>
+      <c r="D13" s="79"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="1"/>
@@ -2145,10 +2145,10 @@
       <c r="J13" s="1"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
-      <c r="M13" s="53"/>
-      <c r="N13" s="54"/>
-      <c r="O13" s="54"/>
-      <c r="P13" s="70"/>
+      <c r="M13" s="63"/>
+      <c r="N13" s="64"/>
+      <c r="O13" s="64"/>
+      <c r="P13" s="80"/>
     </row>
     <row r="14" spans="1:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
@@ -2163,10 +2163,10 @@
       <c r="J14" s="1"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
-      <c r="M14" s="71"/>
-      <c r="N14" s="72"/>
-      <c r="O14" s="72"/>
-      <c r="P14" s="73"/>
+      <c r="M14" s="81"/>
+      <c r="N14" s="82"/>
+      <c r="O14" s="82"/>
+      <c r="P14" s="83"/>
     </row>
     <row r="15" spans="1:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
@@ -2189,10 +2189,10 @@
       <c r="J15" s="1"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
-      <c r="M15" s="71"/>
-      <c r="N15" s="72"/>
-      <c r="O15" s="72"/>
-      <c r="P15" s="73"/>
+      <c r="M15" s="81"/>
+      <c r="N15" s="82"/>
+      <c r="O15" s="82"/>
+      <c r="P15" s="83"/>
     </row>
     <row r="16" spans="1:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
@@ -2207,10 +2207,10 @@
       <c r="J16" s="1"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
-      <c r="M16" s="71"/>
-      <c r="N16" s="72"/>
-      <c r="O16" s="72"/>
-      <c r="P16" s="73"/>
+      <c r="M16" s="81"/>
+      <c r="N16" s="82"/>
+      <c r="O16" s="82"/>
+      <c r="P16" s="83"/>
     </row>
     <row r="17" spans="1:17" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
@@ -2235,10 +2235,10 @@
       <c r="J17" s="1"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
-      <c r="M17" s="74"/>
-      <c r="N17" s="75"/>
-      <c r="O17" s="75"/>
-      <c r="P17" s="76"/>
+      <c r="M17" s="84"/>
+      <c r="N17" s="85"/>
+      <c r="O17" s="85"/>
+      <c r="P17" s="86"/>
     </row>
     <row r="18" spans="1:17" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
@@ -2261,12 +2261,12 @@
       <c r="P18" s="1"/>
     </row>
     <row r="19" spans="1:17" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="79" t="s">
+      <c r="A19" s="89" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="80"/>
-      <c r="C19" s="80"/>
-      <c r="D19" s="81"/>
+      <c r="B19" s="90"/>
+      <c r="C19" s="90"/>
+      <c r="D19" s="91"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="1"/>
@@ -2275,12 +2275,12 @@
       <c r="J19" s="1"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
-      <c r="M19" s="61" t="s">
+      <c r="M19" s="71" t="s">
         <v>29</v>
       </c>
-      <c r="N19" s="82"/>
-      <c r="O19" s="82"/>
-      <c r="P19" s="83"/>
+      <c r="N19" s="92"/>
+      <c r="O19" s="92"/>
+      <c r="P19" s="93"/>
     </row>
     <row r="20" spans="1:17" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
@@ -2301,31 +2301,31 @@
       <c r="J20" s="2"/>
       <c r="K20" s="1"/>
       <c r="L20" s="3"/>
-      <c r="M20" s="90" t="s">
+      <c r="M20" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="N20" s="91"/>
-      <c r="O20" s="91"/>
-      <c r="P20" s="92"/>
+      <c r="N20" s="100"/>
+      <c r="O20" s="100"/>
+      <c r="P20" s="101"/>
     </row>
     <row r="21" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9"/>
-      <c r="B21" s="93">
+      <c r="B21" s="102">
         <v>417589992</v>
       </c>
-      <c r="C21" s="94"/>
-      <c r="D21" s="94"/>
-      <c r="E21" s="58">
+      <c r="C21" s="103"/>
+      <c r="D21" s="103"/>
+      <c r="E21" s="68">
         <v>0</v>
       </c>
-      <c r="F21" s="59"/>
-      <c r="G21" s="60"/>
+      <c r="F21" s="69"/>
+      <c r="G21" s="70"/>
       <c r="H21" s="18"/>
-      <c r="I21" s="58">
+      <c r="I21" s="68">
         <v>0</v>
       </c>
-      <c r="J21" s="59"/>
-      <c r="K21" s="60"/>
+      <c r="J21" s="69"/>
+      <c r="K21" s="70"/>
       <c r="L21" s="3"/>
       <c r="M21" s="7"/>
       <c r="N21" s="8"/>
@@ -2358,22 +2358,22 @@
     </row>
     <row r="23" spans="1:17" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
-      <c r="B23" s="58">
+      <c r="B23" s="68">
         <v>77254149</v>
       </c>
-      <c r="C23" s="59"/>
-      <c r="D23" s="60"/>
-      <c r="E23" s="84">
+      <c r="C23" s="69"/>
+      <c r="D23" s="70"/>
+      <c r="E23" s="61">
         <v>77254149</v>
       </c>
-      <c r="F23" s="85"/>
-      <c r="G23" s="86"/>
+      <c r="F23" s="94"/>
+      <c r="G23" s="95"/>
       <c r="H23" s="18"/>
-      <c r="I23" s="87">
+      <c r="I23" s="96">
         <v>0</v>
       </c>
-      <c r="J23" s="88"/>
-      <c r="K23" s="89"/>
+      <c r="J23" s="97"/>
+      <c r="K23" s="98"/>
       <c r="L23" s="3"/>
       <c r="M23" s="10"/>
       <c r="N23" s="11"/>
@@ -2387,25 +2387,25 @@
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
-      <c r="F25" s="53" t="s">
+      <c r="F25" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="G25" s="54"/>
-      <c r="H25" s="55" t="s">
+      <c r="G25" s="64"/>
+      <c r="H25" s="65" t="s">
         <v>73</v>
       </c>
-      <c r="I25" s="56"/>
-      <c r="J25" s="57"/>
-      <c r="K25" s="55" t="s">
+      <c r="I25" s="66"/>
+      <c r="J25" s="67"/>
+      <c r="K25" s="65" t="s">
         <v>75</v>
       </c>
-      <c r="L25" s="56"/>
-      <c r="M25" s="57"/>
-      <c r="N25" s="55" t="s">
+      <c r="L25" s="66"/>
+      <c r="M25" s="67"/>
+      <c r="N25" s="65" t="s">
         <v>74</v>
       </c>
-      <c r="O25" s="56"/>
-      <c r="P25" s="57"/>
+      <c r="O25" s="66"/>
+      <c r="P25" s="67"/>
       <c r="Q25" s="22"/>
     </row>
     <row r="26" spans="1:17" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2459,31 +2459,31 @@
       </c>
     </row>
     <row r="27" spans="1:17" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="95" t="s">
+      <c r="A27" s="104" t="s">
         <v>82</v>
       </c>
       <c r="B27" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="C27" s="97" t="s">
+      <c r="C27" s="106" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="99" t="s">
+      <c r="D27" s="108" t="s">
         <v>43</v>
       </c>
       <c r="E27" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="97" t="s">
+      <c r="F27" s="106" t="s">
         <v>46</v>
       </c>
-      <c r="G27" s="101" t="s">
+      <c r="G27" s="110" t="s">
         <v>47</v>
       </c>
       <c r="H27" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="I27" s="103" t="s">
+      <c r="I27" s="112" t="s">
         <v>50</v>
       </c>
       <c r="J27" s="46" t="s">
@@ -2492,7 +2492,7 @@
       <c r="K27" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="L27" s="103" t="s">
+      <c r="L27" s="112" t="s">
         <v>55</v>
       </c>
       <c r="M27" s="46" t="s">
@@ -2501,7 +2501,7 @@
       <c r="N27" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="O27" s="103" t="s">
+      <c r="O27" s="112" t="s">
         <v>60</v>
       </c>
       <c r="P27" s="46" t="s">
@@ -2509,35 +2509,35 @@
       </c>
     </row>
     <row r="28" spans="1:17" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="96"/>
+      <c r="A28" s="105"/>
       <c r="B28" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="C28" s="98"/>
-      <c r="D28" s="100"/>
+      <c r="C28" s="107"/>
+      <c r="D28" s="109"/>
       <c r="E28" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="F28" s="98"/>
-      <c r="G28" s="102"/>
+      <c r="F28" s="107"/>
+      <c r="G28" s="111"/>
       <c r="H28" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="I28" s="104"/>
+      <c r="I28" s="113"/>
       <c r="J28" s="47" t="s">
         <v>52</v>
       </c>
       <c r="K28" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="L28" s="104"/>
+      <c r="L28" s="113"/>
       <c r="M28" s="47" t="s">
         <v>57</v>
       </c>
       <c r="N28" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="O28" s="104"/>
+      <c r="O28" s="113"/>
       <c r="P28" s="47" t="s">
         <v>62</v>
       </c>
@@ -2548,44 +2548,44 @@
       </c>
     </row>
     <row r="30" spans="1:17" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="105" t="s">
+      <c r="A30" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="106"/>
-      <c r="C30" s="106"/>
-      <c r="D30" s="106"/>
-      <c r="E30" s="106"/>
-      <c r="F30" s="106"/>
-      <c r="G30" s="106"/>
-      <c r="H30" s="106"/>
-      <c r="I30" s="106"/>
-      <c r="J30" s="106"/>
-      <c r="K30" s="106"/>
-      <c r="L30" s="106"/>
-      <c r="M30" s="106"/>
-      <c r="N30" s="106"/>
-      <c r="O30" s="106"/>
-      <c r="P30" s="107"/>
+      <c r="B30" s="54"/>
+      <c r="C30" s="54"/>
+      <c r="D30" s="54"/>
+      <c r="E30" s="54"/>
+      <c r="F30" s="54"/>
+      <c r="G30" s="54"/>
+      <c r="H30" s="54"/>
+      <c r="I30" s="54"/>
+      <c r="J30" s="54"/>
+      <c r="K30" s="54"/>
+      <c r="L30" s="54"/>
+      <c r="M30" s="54"/>
+      <c r="N30" s="54"/>
+      <c r="O30" s="54"/>
+      <c r="P30" s="55"/>
     </row>
     <row r="31" spans="1:17" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:17" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="108" t="s">
+      <c r="A32" s="56" t="s">
         <v>34</v>
       </c>
       <c r="B32" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="C32" s="108" t="s">
+      <c r="C32" s="56" t="s">
         <v>38</v>
       </c>
       <c r="D32" s="42">
         <v>0.185</v>
       </c>
-      <c r="E32" s="110" t="s">
+      <c r="E32" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="F32" s="111"/>
-      <c r="G32" s="112"/>
+      <c r="F32" s="59"/>
+      <c r="G32" s="60"/>
       <c r="H32" s="48" t="s">
         <v>76</v>
       </c>
@@ -2603,17 +2603,17 @@
       <c r="P32" s="37"/>
     </row>
     <row r="33" spans="1:16" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="109"/>
+      <c r="A33" s="57"/>
       <c r="B33" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="C33" s="109"/>
+      <c r="C33" s="57"/>
       <c r="D33" s="41"/>
-      <c r="E33" s="110" t="s">
+      <c r="E33" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="F33" s="111"/>
-      <c r="G33" s="112"/>
+      <c r="F33" s="59"/>
+      <c r="G33" s="60"/>
       <c r="H33" s="48" t="s">
         <v>77</v>
       </c>
@@ -2631,29 +2631,57 @@
       <c r="P33" s="39"/>
     </row>
     <row r="34" spans="1:16" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="105" t="s">
+      <c r="A34" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="B34" s="106"/>
-      <c r="C34" s="106"/>
-      <c r="D34" s="106"/>
-      <c r="E34" s="106"/>
-      <c r="F34" s="106"/>
-      <c r="G34" s="106"/>
-      <c r="H34" s="106"/>
-      <c r="I34" s="106"/>
-      <c r="J34" s="106"/>
-      <c r="K34" s="106"/>
-      <c r="L34" s="106"/>
-      <c r="M34" s="106"/>
-      <c r="N34" s="107"/>
-      <c r="O34" s="84" t="s">
+      <c r="B34" s="54"/>
+      <c r="C34" s="54"/>
+      <c r="D34" s="54"/>
+      <c r="E34" s="54"/>
+      <c r="F34" s="54"/>
+      <c r="G34" s="54"/>
+      <c r="H34" s="54"/>
+      <c r="I34" s="54"/>
+      <c r="J34" s="54"/>
+      <c r="K34" s="54"/>
+      <c r="L34" s="54"/>
+      <c r="M34" s="54"/>
+      <c r="N34" s="55"/>
+      <c r="O34" s="61" t="s">
         <v>80</v>
       </c>
-      <c r="P34" s="113"/>
+      <c r="P34" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="I27:I28"/>
+    <mergeCell ref="L27:L28"/>
+    <mergeCell ref="O27:O28"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="M19:P19"/>
+    <mergeCell ref="M20:P20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="M11:P11"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="M12:P12"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="M13:P17"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H25:J25"/>
+    <mergeCell ref="K25:M25"/>
+    <mergeCell ref="N25:P25"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="I23:K23"/>
     <mergeCell ref="A30:P30"/>
     <mergeCell ref="A32:A33"/>
     <mergeCell ref="C32:C33"/>
@@ -2661,34 +2689,6 @@
     <mergeCell ref="A34:N34"/>
     <mergeCell ref="E32:G32"/>
     <mergeCell ref="O34:P34"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="H25:J25"/>
-    <mergeCell ref="K25:M25"/>
-    <mergeCell ref="N25:P25"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="M11:P11"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="M12:P12"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="M13:P17"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="M19:P19"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="M20:P20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="I27:I28"/>
-    <mergeCell ref="L27:L28"/>
-    <mergeCell ref="O27:O28"/>
   </mergeCells>
   <phoneticPr fontId="26" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>

</xml_diff>